<commit_message>
v3.0: Implementación de equivalencias
</commit_message>
<xml_diff>
--- a/salida/excel/consumo_horas_educacion_secundaria.xlsx
+++ b/salida/excel/consumo_horas_educacion_secundaria.xlsx
@@ -593,7 +593,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>276.00</t>
+          <t>289.00</t>
         </is>
       </c>
     </row>
@@ -631,7 +631,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>95.00</t>
+          <t>103.00</t>
         </is>
       </c>
     </row>
@@ -643,7 +643,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>148.00</t>
+          <t>150.00</t>
         </is>
       </c>
     </row>
@@ -667,7 +667,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>21.00</t>
+          <t>24.00</t>
         </is>
       </c>
     </row>
@@ -679,7 +679,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>276.00</t>
+          <t>289.00</t>
         </is>
       </c>
     </row>
@@ -1279,12 +1279,12 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>58.00</t>
+          <t>60.00</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>70.00</t>
+          <t>72.00</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -1294,22 +1294,22 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>13.00</t>
+          <t>16.00</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>149.00</t>
+          <t>156.00</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>928.00</t>
+          <t>960.00</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>1120.00</t>
+          <t>1152.00</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
@@ -1319,28 +1319,28 @@
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>208.00</t>
+          <t>256.00</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>2384.00</t>
+          <t>2496.00</t>
         </is>
       </c>
       <c r="Q7" t="n">
+        <v>28</v>
+      </c>
+      <c r="R7" t="n">
         <v>27</v>
-      </c>
-      <c r="R7" t="n">
-        <v>26</v>
       </c>
       <c r="S7" t="n">
         <v>2</v>
       </c>
       <c r="T7" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="U7" t="n">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8">
@@ -1368,12 +1368,12 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>69.00</t>
+          <t>77.00</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>82.00</t>
+          <t>84.00</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -1383,22 +1383,22 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>13.00</t>
+          <t>16.00</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>172.00</t>
+          <t>185.00</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>1104.00</t>
+          <t>1232.00</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>1312.00</t>
+          <t>1344.00</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
@@ -1408,28 +1408,28 @@
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>208.00</t>
+          <t>256.00</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>2752.00</t>
+          <t>2960.00</t>
         </is>
       </c>
       <c r="Q8" t="n">
+        <v>35</v>
+      </c>
+      <c r="R8" t="n">
         <v>32</v>
-      </c>
-      <c r="R8" t="n">
-        <v>31</v>
       </c>
       <c r="S8" t="n">
         <v>2</v>
       </c>
       <c r="T8" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="U8" t="n">
-        <v>71</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9">
@@ -1457,12 +1457,12 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>77.00</t>
+          <t>85.00</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>94.00</t>
+          <t>96.00</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -1472,22 +1472,22 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>13.00</t>
+          <t>16.00</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>196.00</t>
+          <t>209.00</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>1232.00</t>
+          <t>1360.00</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>1504.00</t>
+          <t>1536.00</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
@@ -1497,28 +1497,28 @@
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>208.00</t>
+          <t>256.00</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>3136.00</t>
+          <t>3344.00</t>
         </is>
       </c>
       <c r="Q9" t="n">
+        <v>39</v>
+      </c>
+      <c r="R9" t="n">
         <v>36</v>
-      </c>
-      <c r="R9" t="n">
-        <v>35</v>
       </c>
       <c r="S9" t="n">
         <v>3</v>
       </c>
       <c r="T9" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="U9" t="n">
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10">
@@ -1546,12 +1546,12 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>87.00</t>
+          <t>95.00</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>116.00</t>
+          <t>118.00</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -1561,22 +1561,22 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>17.00</t>
+          <t>20.00</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>232.00</t>
+          <t>245.00</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>1392.00</t>
+          <t>1520.00</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>1856.00</t>
+          <t>1888.00</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
@@ -1586,28 +1586,28 @@
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>272.00</t>
+          <t>320.00</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>3712.00</t>
+          <t>3920.00</t>
         </is>
       </c>
       <c r="Q10" t="n">
+        <v>42</v>
+      </c>
+      <c r="R10" t="n">
         <v>39</v>
-      </c>
-      <c r="R10" t="n">
-        <v>38</v>
       </c>
       <c r="S10" t="n">
         <v>3</v>
       </c>
       <c r="T10" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="U10" t="n">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11">
@@ -1635,12 +1635,12 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>95.00</t>
+          <t>103.00</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>148.00</t>
+          <t>150.00</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -1650,22 +1650,22 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>21.00</t>
+          <t>24.00</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>276.00</t>
+          <t>289.00</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>1520.00</t>
+          <t>1648.00</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>2368.00</t>
+          <t>2400.00</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
@@ -1675,28 +1675,28 @@
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>336.00</t>
+          <t>384.00</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>4416.00</t>
+          <t>4624.00</t>
         </is>
       </c>
       <c r="Q11" t="n">
+        <v>44</v>
+      </c>
+      <c r="R11" t="n">
         <v>41</v>
-      </c>
-      <c r="R11" t="n">
-        <v>40</v>
       </c>
       <c r="S11" t="n">
         <v>3</v>
       </c>
       <c r="T11" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="U11" t="n">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12">
@@ -1724,12 +1724,12 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>95.00</t>
+          <t>103.00</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>148.00</t>
+          <t>150.00</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -1739,22 +1739,22 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>21.00</t>
+          <t>24.00</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>276.00</t>
+          <t>289.00</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>1520.00</t>
+          <t>1648.00</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>2368.00</t>
+          <t>2400.00</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
@@ -1764,28 +1764,28 @@
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>336.00</t>
+          <t>384.00</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>4416.00</t>
+          <t>4624.00</t>
         </is>
       </c>
       <c r="Q12" t="n">
+        <v>44</v>
+      </c>
+      <c r="R12" t="n">
         <v>41</v>
-      </c>
-      <c r="R12" t="n">
-        <v>40</v>
       </c>
       <c r="S12" t="n">
         <v>3</v>
       </c>
       <c r="T12" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="U12" t="n">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13">
@@ -1813,12 +1813,12 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>95.00</t>
+          <t>103.00</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>148.00</t>
+          <t>150.00</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -1828,22 +1828,22 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>21.00</t>
+          <t>24.00</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>276.00</t>
+          <t>289.00</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>1520.00</t>
+          <t>1648.00</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>2368.00</t>
+          <t>2400.00</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
@@ -1853,28 +1853,28 @@
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>336.00</t>
+          <t>384.00</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>4416.00</t>
+          <t>4624.00</t>
         </is>
       </c>
       <c r="Q13" t="n">
+        <v>44</v>
+      </c>
+      <c r="R13" t="n">
         <v>41</v>
-      </c>
-      <c r="R13" t="n">
-        <v>40</v>
       </c>
       <c r="S13" t="n">
         <v>3</v>
       </c>
       <c r="T13" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="U13" t="n">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14">
@@ -1902,12 +1902,12 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>95.00</t>
+          <t>103.00</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>148.00</t>
+          <t>150.00</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1917,22 +1917,22 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>21.00</t>
+          <t>24.00</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>276.00</t>
+          <t>289.00</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>1520.00</t>
+          <t>1648.00</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>2368.00</t>
+          <t>2400.00</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
@@ -1942,28 +1942,28 @@
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>336.00</t>
+          <t>384.00</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>4416.00</t>
+          <t>4624.00</t>
         </is>
       </c>
       <c r="Q14" t="n">
+        <v>44</v>
+      </c>
+      <c r="R14" t="n">
         <v>41</v>
-      </c>
-      <c r="R14" t="n">
-        <v>40</v>
       </c>
       <c r="S14" t="n">
         <v>3</v>
       </c>
       <c r="T14" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="U14" t="n">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15">
@@ -1991,12 +1991,12 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>95.00</t>
+          <t>103.00</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>148.00</t>
+          <t>150.00</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -2006,22 +2006,22 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>21.00</t>
+          <t>24.00</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>276.00</t>
+          <t>289.00</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>1520.00</t>
+          <t>1648.00</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>2368.00</t>
+          <t>2400.00</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
@@ -2031,28 +2031,28 @@
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>336.00</t>
+          <t>384.00</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>4416.00</t>
+          <t>4624.00</t>
         </is>
       </c>
       <c r="Q15" t="n">
+        <v>44</v>
+      </c>
+      <c r="R15" t="n">
         <v>41</v>
-      </c>
-      <c r="R15" t="n">
-        <v>40</v>
       </c>
       <c r="S15" t="n">
         <v>3</v>
       </c>
       <c r="T15" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="U15" t="n">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16">
@@ -2080,12 +2080,12 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>95.00</t>
+          <t>103.00</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>148.00</t>
+          <t>150.00</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -2095,22 +2095,22 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>21.00</t>
+          <t>24.00</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>276.00</t>
+          <t>289.00</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>1520.00</t>
+          <t>1648.00</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>2368.00</t>
+          <t>2400.00</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
@@ -2120,28 +2120,28 @@
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>336.00</t>
+          <t>384.00</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>4416.00</t>
+          <t>4624.00</t>
         </is>
       </c>
       <c r="Q16" t="n">
+        <v>44</v>
+      </c>
+      <c r="R16" t="n">
         <v>41</v>
-      </c>
-      <c r="R16" t="n">
-        <v>40</v>
       </c>
       <c r="S16" t="n">
         <v>3</v>
       </c>
       <c r="T16" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="U16" t="n">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17">
@@ -2169,12 +2169,12 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>95.00</t>
+          <t>103.00</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>148.00</t>
+          <t>150.00</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -2184,22 +2184,22 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>21.00</t>
+          <t>24.00</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>276.00</t>
+          <t>289.00</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>1520.00</t>
+          <t>1648.00</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>2368.00</t>
+          <t>2400.00</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
@@ -2209,28 +2209,28 @@
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>336.00</t>
+          <t>384.00</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>4416.00</t>
+          <t>4624.00</t>
         </is>
       </c>
       <c r="Q17" t="n">
+        <v>44</v>
+      </c>
+      <c r="R17" t="n">
         <v>41</v>
-      </c>
-      <c r="R17" t="n">
-        <v>40</v>
       </c>
       <c r="S17" t="n">
         <v>3</v>
       </c>
       <c r="T17" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="U17" t="n">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18">
@@ -2258,12 +2258,12 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>95.00</t>
+          <t>103.00</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>148.00</t>
+          <t>150.00</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -2273,22 +2273,22 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>21.00</t>
+          <t>24.00</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>276.00</t>
+          <t>289.00</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>1520.00</t>
+          <t>1648.00</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>2368.00</t>
+          <t>2400.00</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
@@ -2298,28 +2298,28 @@
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>336.00</t>
+          <t>384.00</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>4416.00</t>
+          <t>4624.00</t>
         </is>
       </c>
       <c r="Q18" t="n">
+        <v>44</v>
+      </c>
+      <c r="R18" t="n">
         <v>41</v>
-      </c>
-      <c r="R18" t="n">
-        <v>40</v>
       </c>
       <c r="S18" t="n">
         <v>3</v>
       </c>
       <c r="T18" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="U18" t="n">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19">
@@ -2347,12 +2347,12 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>95.00</t>
+          <t>103.00</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>148.00</t>
+          <t>150.00</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -2362,22 +2362,22 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>21.00</t>
+          <t>24.00</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>276.00</t>
+          <t>289.00</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>1520.00</t>
+          <t>1648.00</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>2368.00</t>
+          <t>2400.00</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
@@ -2387,28 +2387,28 @@
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>336.00</t>
+          <t>384.00</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>4416.00</t>
+          <t>4624.00</t>
         </is>
       </c>
       <c r="Q19" t="n">
+        <v>44</v>
+      </c>
+      <c r="R19" t="n">
         <v>41</v>
-      </c>
-      <c r="R19" t="n">
-        <v>40</v>
       </c>
       <c r="S19" t="n">
         <v>3</v>
       </c>
       <c r="T19" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="U19" t="n">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20">
@@ -2436,12 +2436,12 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>95.00</t>
+          <t>103.00</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>148.00</t>
+          <t>150.00</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -2451,22 +2451,22 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>21.00</t>
+          <t>24.00</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>276.00</t>
+          <t>289.00</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>1520.00</t>
+          <t>1648.00</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>2368.00</t>
+          <t>2400.00</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
@@ -2476,28 +2476,28 @@
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>336.00</t>
+          <t>384.00</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>4416.00</t>
+          <t>4624.00</t>
         </is>
       </c>
       <c r="Q20" t="n">
+        <v>44</v>
+      </c>
+      <c r="R20" t="n">
         <v>41</v>
-      </c>
-      <c r="R20" t="n">
-        <v>40</v>
       </c>
       <c r="S20" t="n">
         <v>3</v>
       </c>
       <c r="T20" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="U20" t="n">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21">
@@ -2525,12 +2525,12 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>95.00</t>
+          <t>103.00</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>148.00</t>
+          <t>150.00</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -2540,22 +2540,22 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>21.00</t>
+          <t>24.00</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>276.00</t>
+          <t>289.00</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>1520.00</t>
+          <t>1648.00</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>2368.00</t>
+          <t>2400.00</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
@@ -2565,28 +2565,28 @@
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>336.00</t>
+          <t>384.00</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>4416.00</t>
+          <t>4624.00</t>
         </is>
       </c>
       <c r="Q21" t="n">
+        <v>44</v>
+      </c>
+      <c r="R21" t="n">
         <v>41</v>
-      </c>
-      <c r="R21" t="n">
-        <v>40</v>
       </c>
       <c r="S21" t="n">
         <v>3</v>
       </c>
       <c r="T21" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="U21" t="n">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -3085,7 +3085,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2.57</t>
+          <t>2.58</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -3101,27 +3101,27 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>28.50</t>
+          <t>33.75</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
+          <t>16.50</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>48.9%</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
           <t>15.00</t>
         </is>
       </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>52.6%</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>13.50</t>
-        </is>
-      </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>47.4%</t>
+          <t>44.4%</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
@@ -3136,12 +3136,12 @@
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>2.25</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>6.7%</t>
         </is>
       </c>
     </row>
@@ -3160,7 +3160,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.98</t>
+          <t>1.99</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -3176,17 +3176,17 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>16.10</t>
+          <t>20.30</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>7.70</t>
+          <t>11.90</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>47.8%</t>
+          <t>58.6%</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
@@ -3196,7 +3196,7 @@
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>52.2%</t>
+          <t>41.4%</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
@@ -3621,12 +3621,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1536.00</t>
+          <t>1568.00</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1952.00</t>
+          <t>1984.00</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -3636,12 +3636,12 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>416.00</t>
+          <t>464.00</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>4160.00</t>
+          <t>4272.00</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -3651,12 +3651,12 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>149.00</t>
+          <t>156.00</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>130.00</t>
+          <t>133.50</t>
         </is>
       </c>
     </row>
@@ -3669,12 +3669,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2336.00</t>
+          <t>2592.00</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2816.00</t>
+          <t>2880.00</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -3684,27 +3684,27 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>416.00</t>
+          <t>512.00</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>5888.00</t>
+          <t>6304.00</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>172.00</t>
+          <t>185.00</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>196.00</t>
+          <t>209.00</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>184.00</t>
+          <t>197.00</t>
         </is>
       </c>
     </row>
@@ -3717,12 +3717,12 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2912.00</t>
+          <t>3168.00</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>4224.00</t>
+          <t>4288.00</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -3732,27 +3732,27 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>608.00</t>
+          <t>704.00</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>8128.00</t>
+          <t>8544.00</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>232.00</t>
+          <t>245.00</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>276.00</t>
+          <t>289.00</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>254.00</t>
+          <t>267.00</t>
         </is>
       </c>
     </row>
@@ -3765,12 +3765,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>3040.00</t>
+          <t>3296.00</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>4736.00</t>
+          <t>4800.00</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -3780,27 +3780,27 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>672.00</t>
+          <t>768.00</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>8832.00</t>
+          <t>9248.00</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>276.00</t>
+          <t>289.00</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>276.00</t>
+          <t>289.00</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>276.00</t>
+          <t>289.00</t>
         </is>
       </c>
     </row>
@@ -3813,12 +3813,12 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>3040.00</t>
+          <t>3296.00</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>4736.00</t>
+          <t>4800.00</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -3828,27 +3828,27 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>672.00</t>
+          <t>768.00</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>8832.00</t>
+          <t>9248.00</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>276.00</t>
+          <t>289.00</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>276.00</t>
+          <t>289.00</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>276.00</t>
+          <t>289.00</t>
         </is>
       </c>
     </row>
@@ -3861,12 +3861,12 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>3040.00</t>
+          <t>3296.00</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>4736.00</t>
+          <t>4800.00</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -3876,27 +3876,27 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>672.00</t>
+          <t>768.00</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>8832.00</t>
+          <t>9248.00</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>276.00</t>
+          <t>289.00</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>276.00</t>
+          <t>289.00</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>276.00</t>
+          <t>289.00</t>
         </is>
       </c>
     </row>
@@ -3909,12 +3909,12 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>3040.00</t>
+          <t>3296.00</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>4736.00</t>
+          <t>4800.00</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -3924,27 +3924,27 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>672.00</t>
+          <t>768.00</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>8832.00</t>
+          <t>9248.00</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>276.00</t>
+          <t>289.00</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>276.00</t>
+          <t>289.00</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>276.00</t>
+          <t>289.00</t>
         </is>
       </c>
     </row>
@@ -3957,12 +3957,12 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>3040.00</t>
+          <t>3296.00</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>4736.00</t>
+          <t>4800.00</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -3972,27 +3972,27 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>672.00</t>
+          <t>768.00</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>8832.00</t>
+          <t>9248.00</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>276.00</t>
+          <t>289.00</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>276.00</t>
+          <t>289.00</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>276.00</t>
+          <t>289.00</t>
         </is>
       </c>
     </row>
@@ -4164,19 +4164,19 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C7" t="n">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D7" t="n">
         <v>8</v>
       </c>
       <c r="E7" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F7" t="n">
-        <v>149</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8">
@@ -4186,19 +4186,19 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="C8" t="n">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D8" t="n">
         <v>8</v>
       </c>
       <c r="E8" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F8" t="n">
-        <v>172</v>
+        <v>185</v>
       </c>
     </row>
     <row r="9">
@@ -4208,19 +4208,19 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C9" t="n">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D9" t="n">
         <v>12</v>
       </c>
       <c r="E9" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F9" t="n">
-        <v>196</v>
+        <v>209</v>
       </c>
     </row>
     <row r="10">
@@ -4230,19 +4230,19 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="C10" t="n">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D10" t="n">
         <v>12</v>
       </c>
       <c r="E10" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F10" t="n">
-        <v>232</v>
+        <v>245</v>
       </c>
     </row>
     <row r="11">
@@ -4252,19 +4252,19 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="C11" t="n">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D11" t="n">
         <v>12</v>
       </c>
       <c r="E11" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F11" t="n">
-        <v>276</v>
+        <v>289</v>
       </c>
     </row>
     <row r="12">
@@ -4274,19 +4274,19 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="C12" t="n">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D12" t="n">
         <v>12</v>
       </c>
       <c r="E12" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F12" t="n">
-        <v>276</v>
+        <v>289</v>
       </c>
     </row>
     <row r="13">
@@ -4296,19 +4296,19 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="C13" t="n">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D13" t="n">
         <v>12</v>
       </c>
       <c r="E13" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F13" t="n">
-        <v>276</v>
+        <v>289</v>
       </c>
     </row>
     <row r="14">
@@ -4318,19 +4318,19 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="C14" t="n">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D14" t="n">
         <v>12</v>
       </c>
       <c r="E14" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F14" t="n">
-        <v>276</v>
+        <v>289</v>
       </c>
     </row>
     <row r="15">
@@ -4340,19 +4340,19 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="C15" t="n">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D15" t="n">
         <v>12</v>
       </c>
       <c r="E15" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F15" t="n">
-        <v>276</v>
+        <v>289</v>
       </c>
     </row>
     <row r="16">
@@ -4362,19 +4362,19 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="C16" t="n">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D16" t="n">
         <v>12</v>
       </c>
       <c r="E16" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F16" t="n">
-        <v>276</v>
+        <v>289</v>
       </c>
     </row>
     <row r="17">
@@ -4384,19 +4384,19 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="C17" t="n">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D17" t="n">
         <v>12</v>
       </c>
       <c r="E17" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F17" t="n">
-        <v>276</v>
+        <v>289</v>
       </c>
     </row>
     <row r="18">
@@ -4406,19 +4406,19 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="C18" t="n">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D18" t="n">
         <v>12</v>
       </c>
       <c r="E18" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F18" t="n">
-        <v>276</v>
+        <v>289</v>
       </c>
     </row>
     <row r="19">
@@ -4428,19 +4428,19 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="C19" t="n">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D19" t="n">
         <v>12</v>
       </c>
       <c r="E19" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F19" t="n">
-        <v>276</v>
+        <v>289</v>
       </c>
     </row>
     <row r="20">
@@ -4450,19 +4450,19 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="C20" t="n">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D20" t="n">
         <v>12</v>
       </c>
       <c r="E20" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F20" t="n">
-        <v>276</v>
+        <v>289</v>
       </c>
     </row>
     <row r="21">
@@ -4472,19 +4472,19 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="C21" t="n">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D21" t="n">
         <v>12</v>
       </c>
       <c r="E21" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F21" t="n">
-        <v>276</v>
+        <v>289</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v4: Tabla Pivote con laboratorios especificos
</commit_message>
<xml_diff>
--- a/salida/excel/consumo_horas_educacion_secundaria.xlsx
+++ b/salida/excel/consumo_horas_educacion_secundaria.xlsx
@@ -593,7 +593,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>289.00</t>
+          <t>284.00</t>
         </is>
       </c>
     </row>
@@ -631,7 +631,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>103.00</t>
+          <t>236.00</t>
         </is>
       </c>
     </row>
@@ -643,7 +643,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>150.00</t>
+          <t>12.00</t>
         </is>
       </c>
     </row>
@@ -679,7 +679,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>289.00</t>
+          <t>284.00</t>
         </is>
       </c>
     </row>
@@ -834,12 +834,12 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2.00</t>
+          <t>4.00</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -859,12 +859,12 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>32.00</t>
+          <t>64.00</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>32.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
@@ -883,10 +883,10 @@
         </is>
       </c>
       <c r="Q2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S2" t="n">
         <v>1</v>
@@ -923,12 +923,12 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>14.00</t>
+          <t>26.00</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>16.00</t>
+          <t>4.00</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -948,12 +948,12 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>224.00</t>
+          <t>416.00</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>256.00</t>
+          <t>64.00</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
@@ -972,10 +972,10 @@
         </is>
       </c>
       <c r="Q3" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="R3" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="S3" t="n">
         <v>1</v>
@@ -1012,12 +1012,12 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>21.00</t>
+          <t>43.00</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>26.00</t>
+          <t>4.00</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -1037,12 +1037,12 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>336.00</t>
+          <t>688.00</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>416.00</t>
+          <t>64.00</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
@@ -1061,10 +1061,10 @@
         </is>
       </c>
       <c r="Q4" t="n">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="R4" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="S4" t="n">
         <v>2</v>
@@ -1101,12 +1101,12 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>32.00</t>
+          <t>62.00</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>38.00</t>
+          <t>8.00</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -1126,12 +1126,12 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>512.00</t>
+          <t>992.00</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>608.00</t>
+          <t>128.00</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
@@ -1150,10 +1150,10 @@
         </is>
       </c>
       <c r="Q5" t="n">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="R5" t="n">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="S5" t="n">
         <v>2</v>
@@ -1190,12 +1190,12 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>38.00</t>
+          <t>78.00</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>52.00</t>
+          <t>12.00</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -1215,12 +1215,12 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>608.00</t>
+          <t>1248.00</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>832.00</t>
+          <t>192.00</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
@@ -1239,10 +1239,10 @@
         </is>
       </c>
       <c r="Q6" t="n">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="R6" t="n">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="S6" t="n">
         <v>2</v>
@@ -1279,12 +1279,12 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>60.00</t>
+          <t>120.00</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>72.00</t>
+          <t>12.00</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -1304,12 +1304,12 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>960.00</t>
+          <t>1920.00</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>1152.00</t>
+          <t>192.00</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
@@ -1328,10 +1328,10 @@
         </is>
       </c>
       <c r="Q7" t="n">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="R7" t="n">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="S7" t="n">
         <v>2</v>
@@ -1368,12 +1368,12 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>77.00</t>
+          <t>149.00</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>84.00</t>
+          <t>12.00</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -1393,12 +1393,12 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>1232.00</t>
+          <t>2384.00</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>1344.00</t>
+          <t>192.00</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
@@ -1417,10 +1417,10 @@
         </is>
       </c>
       <c r="Q8" t="n">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="R8" t="n">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="S8" t="n">
         <v>2</v>
@@ -1457,12 +1457,12 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>85.00</t>
+          <t>164.00</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>96.00</t>
+          <t>12.00</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -1477,17 +1477,17 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>209.00</t>
+          <t>204.00</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>1360.00</t>
+          <t>2624.00</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>1536.00</t>
+          <t>192.00</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
@@ -1502,14 +1502,14 @@
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>3344.00</t>
+          <t>3264.00</t>
         </is>
       </c>
       <c r="Q9" t="n">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="R9" t="n">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="S9" t="n">
         <v>3</v>
@@ -1546,12 +1546,12 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>95.00</t>
+          <t>196.00</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>118.00</t>
+          <t>12.00</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -1566,17 +1566,17 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>245.00</t>
+          <t>240.00</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>1520.00</t>
+          <t>3136.00</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>1888.00</t>
+          <t>192.00</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
@@ -1591,14 +1591,14 @@
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>3920.00</t>
+          <t>3840.00</t>
         </is>
       </c>
       <c r="Q10" t="n">
-        <v>42</v>
+        <v>78</v>
       </c>
       <c r="R10" t="n">
-        <v>39</v>
+        <v>3</v>
       </c>
       <c r="S10" t="n">
         <v>3</v>
@@ -1635,12 +1635,12 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>103.00</t>
+          <t>236.00</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>150.00</t>
+          <t>12.00</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -1655,17 +1655,17 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>289.00</t>
+          <t>284.00</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>1648.00</t>
+          <t>3776.00</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>2400.00</t>
+          <t>192.00</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
@@ -1680,14 +1680,14 @@
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>4624.00</t>
+          <t>4544.00</t>
         </is>
       </c>
       <c r="Q11" t="n">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="R11" t="n">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="S11" t="n">
         <v>3</v>
@@ -1724,12 +1724,12 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>103.00</t>
+          <t>236.00</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>150.00</t>
+          <t>12.00</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -1744,17 +1744,17 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>289.00</t>
+          <t>284.00</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>1648.00</t>
+          <t>3776.00</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>2400.00</t>
+          <t>192.00</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
@@ -1769,14 +1769,14 @@
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>4624.00</t>
+          <t>4544.00</t>
         </is>
       </c>
       <c r="Q12" t="n">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="R12" t="n">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="S12" t="n">
         <v>3</v>
@@ -1813,12 +1813,12 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>103.00</t>
+          <t>236.00</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>150.00</t>
+          <t>12.00</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -1833,17 +1833,17 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>289.00</t>
+          <t>284.00</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>1648.00</t>
+          <t>3776.00</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>2400.00</t>
+          <t>192.00</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
@@ -1858,14 +1858,14 @@
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>4624.00</t>
+          <t>4544.00</t>
         </is>
       </c>
       <c r="Q13" t="n">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="R13" t="n">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="S13" t="n">
         <v>3</v>
@@ -1902,12 +1902,12 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>103.00</t>
+          <t>236.00</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>150.00</t>
+          <t>12.00</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1922,17 +1922,17 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>289.00</t>
+          <t>284.00</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>1648.00</t>
+          <t>3776.00</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>2400.00</t>
+          <t>192.00</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
@@ -1947,14 +1947,14 @@
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>4624.00</t>
+          <t>4544.00</t>
         </is>
       </c>
       <c r="Q14" t="n">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="R14" t="n">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="S14" t="n">
         <v>3</v>
@@ -1991,12 +1991,12 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>103.00</t>
+          <t>236.00</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>150.00</t>
+          <t>12.00</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -2011,17 +2011,17 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>289.00</t>
+          <t>284.00</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>1648.00</t>
+          <t>3776.00</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>2400.00</t>
+          <t>192.00</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
@@ -2036,14 +2036,14 @@
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>4624.00</t>
+          <t>4544.00</t>
         </is>
       </c>
       <c r="Q15" t="n">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="R15" t="n">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="S15" t="n">
         <v>3</v>
@@ -2080,12 +2080,12 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>103.00</t>
+          <t>236.00</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>150.00</t>
+          <t>12.00</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -2100,17 +2100,17 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>289.00</t>
+          <t>284.00</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>1648.00</t>
+          <t>3776.00</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>2400.00</t>
+          <t>192.00</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
@@ -2125,14 +2125,14 @@
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>4624.00</t>
+          <t>4544.00</t>
         </is>
       </c>
       <c r="Q16" t="n">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="R16" t="n">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="S16" t="n">
         <v>3</v>
@@ -2169,12 +2169,12 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>103.00</t>
+          <t>236.00</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>150.00</t>
+          <t>12.00</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -2189,17 +2189,17 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>289.00</t>
+          <t>284.00</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>1648.00</t>
+          <t>3776.00</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>2400.00</t>
+          <t>192.00</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
@@ -2214,14 +2214,14 @@
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>4624.00</t>
+          <t>4544.00</t>
         </is>
       </c>
       <c r="Q17" t="n">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="R17" t="n">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="S17" t="n">
         <v>3</v>
@@ -2258,12 +2258,12 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>103.00</t>
+          <t>236.00</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>150.00</t>
+          <t>12.00</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -2278,17 +2278,17 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>289.00</t>
+          <t>284.00</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>1648.00</t>
+          <t>3776.00</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>2400.00</t>
+          <t>192.00</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
@@ -2303,14 +2303,14 @@
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>4624.00</t>
+          <t>4544.00</t>
         </is>
       </c>
       <c r="Q18" t="n">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="R18" t="n">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="S18" t="n">
         <v>3</v>
@@ -2347,12 +2347,12 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>103.00</t>
+          <t>236.00</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>150.00</t>
+          <t>12.00</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -2367,17 +2367,17 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>289.00</t>
+          <t>284.00</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>1648.00</t>
+          <t>3776.00</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>2400.00</t>
+          <t>192.00</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
@@ -2392,14 +2392,14 @@
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>4624.00</t>
+          <t>4544.00</t>
         </is>
       </c>
       <c r="Q19" t="n">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="R19" t="n">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="S19" t="n">
         <v>3</v>
@@ -2436,12 +2436,12 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>103.00</t>
+          <t>236.00</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>150.00</t>
+          <t>12.00</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -2456,17 +2456,17 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>289.00</t>
+          <t>284.00</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>1648.00</t>
+          <t>3776.00</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>2400.00</t>
+          <t>192.00</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
@@ -2481,14 +2481,14 @@
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>4624.00</t>
+          <t>4544.00</t>
         </is>
       </c>
       <c r="Q20" t="n">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="R20" t="n">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="S20" t="n">
         <v>3</v>
@@ -2525,12 +2525,12 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>103.00</t>
+          <t>236.00</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>150.00</t>
+          <t>12.00</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -2545,17 +2545,17 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>289.00</t>
+          <t>284.00</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>1648.00</t>
+          <t>3776.00</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>2400.00</t>
+          <t>192.00</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
@@ -2570,14 +2570,14 @@
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>4624.00</t>
+          <t>4544.00</t>
         </is>
       </c>
       <c r="Q21" t="n">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="R21" t="n">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="S21" t="n">
         <v>3</v>
@@ -2731,32 +2731,32 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>2.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>25.0%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>2.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>25.0%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>4.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>50.0%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
@@ -2806,22 +2806,22 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>11.40</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>41.4%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>13.30</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>48.3%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
@@ -2836,12 +2836,12 @@
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>2.85</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>10.3%</t>
+          <t>0.0%</t>
         </is>
       </c>
     </row>
@@ -2881,42 +2881,42 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>6.30</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>26.9%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>9.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>38.5%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>3.60</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>15.4%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>4.50</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>19.2%</t>
+          <t>0.0%</t>
         </is>
       </c>
     </row>
@@ -2956,22 +2956,22 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>9.35</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>39.3%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>10.20</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>42.9%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
@@ -2986,12 +2986,12 @@
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>4.25</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>17.9%</t>
+          <t>0.0%</t>
         </is>
       </c>
     </row>
@@ -3031,22 +3031,22 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>4.80</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>30.0%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>11.20</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>70.0%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
@@ -3106,22 +3106,22 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>16.50</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>48.9%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>15.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>44.4%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
@@ -3136,12 +3136,12 @@
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>2.25</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>6.7%</t>
+          <t>0.0%</t>
         </is>
       </c>
     </row>
@@ -3181,22 +3181,22 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>11.90</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>58.6%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>8.40</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>41.4%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
@@ -3251,37 +3251,37 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>15.60</t>
+          <t>12.35</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>5.20</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>33.3%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>7.80</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>50.0%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>2.60</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>16.7%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
@@ -3331,22 +3331,22 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>6.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>27.8%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>13.20</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>61.1%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
@@ -3361,12 +3361,12 @@
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>2.40</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>11.1%</t>
+          <t>0.0%</t>
         </is>
       </c>
     </row>
@@ -3406,22 +3406,22 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>4.40</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>18.2%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>17.60</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>72.7%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
@@ -3436,12 +3436,12 @@
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>2.20</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>9.1%</t>
+          <t>0.0%</t>
         </is>
       </c>
     </row>
@@ -3525,27 +3525,27 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>256.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>288.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>128.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>48.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>720.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -3573,27 +3573,27 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>848.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1024.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>256.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>336.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2464.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -3621,27 +3621,27 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1568.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1984.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>256.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>464.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>4272.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -3669,27 +3669,27 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2592.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2880.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>320.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>512.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>6304.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -3699,12 +3699,12 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>209.00</t>
+          <t>204.00</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>197.00</t>
+          <t>194.50</t>
         </is>
       </c>
     </row>
@@ -3717,42 +3717,42 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>3168.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>4288.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>384.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>704.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>8544.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>245.00</t>
+          <t>240.00</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>289.00</t>
+          <t>284.00</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>267.00</t>
+          <t>262.00</t>
         </is>
       </c>
     </row>
@@ -3765,42 +3765,42 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>3296.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>4800.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>384.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>768.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>9248.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>289.00</t>
+          <t>284.00</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>289.00</t>
+          <t>284.00</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>289.00</t>
+          <t>284.00</t>
         </is>
       </c>
     </row>
@@ -3813,42 +3813,42 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>3296.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>4800.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>384.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>768.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>9248.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>289.00</t>
+          <t>284.00</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>289.00</t>
+          <t>284.00</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>289.00</t>
+          <t>284.00</t>
         </is>
       </c>
     </row>
@@ -3861,42 +3861,42 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>3296.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>4800.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>384.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>768.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>9248.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>289.00</t>
+          <t>284.00</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>289.00</t>
+          <t>284.00</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>289.00</t>
+          <t>284.00</t>
         </is>
       </c>
     </row>
@@ -3909,42 +3909,42 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>3296.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>4800.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>384.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>768.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>9248.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>289.00</t>
+          <t>284.00</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>289.00</t>
+          <t>284.00</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>289.00</t>
+          <t>284.00</t>
         </is>
       </c>
     </row>
@@ -3957,42 +3957,42 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>3296.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>4800.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>384.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>768.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>9248.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>289.00</t>
+          <t>284.00</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>289.00</t>
+          <t>284.00</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>289.00</t>
+          <t>284.00</t>
         </is>
       </c>
     </row>
@@ -4007,7 +4007,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4028,20 +4028,25 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Laboratorio</t>
+          <t>Laboratorio de Computadoras</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Laboratorio de Química</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Taller</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Virtual</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
@@ -4054,18 +4059,21 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
         <v>4</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>0</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>8</v>
       </c>
     </row>
@@ -4076,18 +4084,21 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="C3" t="n">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
         <v>4</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>3</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>37</v>
       </c>
     </row>
@@ -4098,18 +4109,21 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="C4" t="n">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="D4" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
         <v>8</v>
       </c>
       <c r="F4" t="n">
+        <v>8</v>
+      </c>
+      <c r="G4" t="n">
         <v>63</v>
       </c>
     </row>
@@ -4120,18 +4134,21 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="C5" t="n">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="D5" t="n">
+        <v>4</v>
+      </c>
+      <c r="E5" t="n">
         <v>8</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>13</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>91</v>
       </c>
     </row>
@@ -4142,18 +4159,21 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>38</v>
+        <v>78</v>
       </c>
       <c r="C6" t="n">
-        <v>52</v>
+        <v>4</v>
       </c>
       <c r="D6" t="n">
         <v>8</v>
       </c>
       <c r="E6" t="n">
+        <v>8</v>
+      </c>
+      <c r="F6" t="n">
         <v>13</v>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
         <v>111</v>
       </c>
     </row>
@@ -4164,18 +4184,21 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="C7" t="n">
-        <v>72</v>
+        <v>4</v>
       </c>
       <c r="D7" t="n">
         <v>8</v>
       </c>
       <c r="E7" t="n">
+        <v>8</v>
+      </c>
+      <c r="F7" t="n">
         <v>16</v>
       </c>
-      <c r="F7" t="n">
+      <c r="G7" t="n">
         <v>156</v>
       </c>
     </row>
@@ -4186,18 +4209,21 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>77</v>
+        <v>149</v>
       </c>
       <c r="C8" t="n">
-        <v>84</v>
+        <v>4</v>
       </c>
       <c r="D8" t="n">
         <v>8</v>
       </c>
       <c r="E8" t="n">
+        <v>8</v>
+      </c>
+      <c r="F8" t="n">
         <v>16</v>
       </c>
-      <c r="F8" t="n">
+      <c r="G8" t="n">
         <v>185</v>
       </c>
     </row>
@@ -4208,19 +4234,22 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>85</v>
+        <v>164</v>
       </c>
       <c r="C9" t="n">
-        <v>96</v>
+        <v>4</v>
       </c>
       <c r="D9" t="n">
+        <v>8</v>
+      </c>
+      <c r="E9" t="n">
         <v>12</v>
       </c>
-      <c r="E9" t="n">
+      <c r="F9" t="n">
         <v>16</v>
       </c>
-      <c r="F9" t="n">
-        <v>209</v>
+      <c r="G9" t="n">
+        <v>204</v>
       </c>
     </row>
     <row r="10">
@@ -4230,19 +4259,22 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>95</v>
+        <v>196</v>
       </c>
       <c r="C10" t="n">
-        <v>118</v>
+        <v>4</v>
       </c>
       <c r="D10" t="n">
+        <v>8</v>
+      </c>
+      <c r="E10" t="n">
         <v>12</v>
       </c>
-      <c r="E10" t="n">
+      <c r="F10" t="n">
         <v>20</v>
       </c>
-      <c r="F10" t="n">
-        <v>245</v>
+      <c r="G10" t="n">
+        <v>240</v>
       </c>
     </row>
     <row r="11">
@@ -4252,19 +4284,22 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>103</v>
+        <v>236</v>
       </c>
       <c r="C11" t="n">
-        <v>150</v>
+        <v>4</v>
       </c>
       <c r="D11" t="n">
+        <v>8</v>
+      </c>
+      <c r="E11" t="n">
         <v>12</v>
       </c>
-      <c r="E11" t="n">
+      <c r="F11" t="n">
         <v>24</v>
       </c>
-      <c r="F11" t="n">
-        <v>289</v>
+      <c r="G11" t="n">
+        <v>284</v>
       </c>
     </row>
     <row r="12">
@@ -4274,19 +4309,22 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>103</v>
+        <v>236</v>
       </c>
       <c r="C12" t="n">
-        <v>150</v>
+        <v>4</v>
       </c>
       <c r="D12" t="n">
+        <v>8</v>
+      </c>
+      <c r="E12" t="n">
         <v>12</v>
       </c>
-      <c r="E12" t="n">
+      <c r="F12" t="n">
         <v>24</v>
       </c>
-      <c r="F12" t="n">
-        <v>289</v>
+      <c r="G12" t="n">
+        <v>284</v>
       </c>
     </row>
     <row r="13">
@@ -4296,19 +4334,22 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>103</v>
+        <v>236</v>
       </c>
       <c r="C13" t="n">
-        <v>150</v>
+        <v>4</v>
       </c>
       <c r="D13" t="n">
+        <v>8</v>
+      </c>
+      <c r="E13" t="n">
         <v>12</v>
       </c>
-      <c r="E13" t="n">
+      <c r="F13" t="n">
         <v>24</v>
       </c>
-      <c r="F13" t="n">
-        <v>289</v>
+      <c r="G13" t="n">
+        <v>284</v>
       </c>
     </row>
     <row r="14">
@@ -4318,19 +4359,22 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>103</v>
+        <v>236</v>
       </c>
       <c r="C14" t="n">
-        <v>150</v>
+        <v>4</v>
       </c>
       <c r="D14" t="n">
+        <v>8</v>
+      </c>
+      <c r="E14" t="n">
         <v>12</v>
       </c>
-      <c r="E14" t="n">
+      <c r="F14" t="n">
         <v>24</v>
       </c>
-      <c r="F14" t="n">
-        <v>289</v>
+      <c r="G14" t="n">
+        <v>284</v>
       </c>
     </row>
     <row r="15">
@@ -4340,19 +4384,22 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>103</v>
+        <v>236</v>
       </c>
       <c r="C15" t="n">
-        <v>150</v>
+        <v>4</v>
       </c>
       <c r="D15" t="n">
+        <v>8</v>
+      </c>
+      <c r="E15" t="n">
         <v>12</v>
       </c>
-      <c r="E15" t="n">
+      <c r="F15" t="n">
         <v>24</v>
       </c>
-      <c r="F15" t="n">
-        <v>289</v>
+      <c r="G15" t="n">
+        <v>284</v>
       </c>
     </row>
     <row r="16">
@@ -4362,19 +4409,22 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>103</v>
+        <v>236</v>
       </c>
       <c r="C16" t="n">
-        <v>150</v>
+        <v>4</v>
       </c>
       <c r="D16" t="n">
+        <v>8</v>
+      </c>
+      <c r="E16" t="n">
         <v>12</v>
       </c>
-      <c r="E16" t="n">
+      <c r="F16" t="n">
         <v>24</v>
       </c>
-      <c r="F16" t="n">
-        <v>289</v>
+      <c r="G16" t="n">
+        <v>284</v>
       </c>
     </row>
     <row r="17">
@@ -4384,19 +4434,22 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>103</v>
+        <v>236</v>
       </c>
       <c r="C17" t="n">
-        <v>150</v>
+        <v>4</v>
       </c>
       <c r="D17" t="n">
+        <v>8</v>
+      </c>
+      <c r="E17" t="n">
         <v>12</v>
       </c>
-      <c r="E17" t="n">
+      <c r="F17" t="n">
         <v>24</v>
       </c>
-      <c r="F17" t="n">
-        <v>289</v>
+      <c r="G17" t="n">
+        <v>284</v>
       </c>
     </row>
     <row r="18">
@@ -4406,19 +4459,22 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>103</v>
+        <v>236</v>
       </c>
       <c r="C18" t="n">
-        <v>150</v>
+        <v>4</v>
       </c>
       <c r="D18" t="n">
+        <v>8</v>
+      </c>
+      <c r="E18" t="n">
         <v>12</v>
       </c>
-      <c r="E18" t="n">
+      <c r="F18" t="n">
         <v>24</v>
       </c>
-      <c r="F18" t="n">
-        <v>289</v>
+      <c r="G18" t="n">
+        <v>284</v>
       </c>
     </row>
     <row r="19">
@@ -4428,19 +4484,22 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>103</v>
+        <v>236</v>
       </c>
       <c r="C19" t="n">
-        <v>150</v>
+        <v>4</v>
       </c>
       <c r="D19" t="n">
+        <v>8</v>
+      </c>
+      <c r="E19" t="n">
         <v>12</v>
       </c>
-      <c r="E19" t="n">
+      <c r="F19" t="n">
         <v>24</v>
       </c>
-      <c r="F19" t="n">
-        <v>289</v>
+      <c r="G19" t="n">
+        <v>284</v>
       </c>
     </row>
     <row r="20">
@@ -4450,19 +4509,22 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>103</v>
+        <v>236</v>
       </c>
       <c r="C20" t="n">
-        <v>150</v>
+        <v>4</v>
       </c>
       <c r="D20" t="n">
+        <v>8</v>
+      </c>
+      <c r="E20" t="n">
         <v>12</v>
       </c>
-      <c r="E20" t="n">
+      <c r="F20" t="n">
         <v>24</v>
       </c>
-      <c r="F20" t="n">
-        <v>289</v>
+      <c r="G20" t="n">
+        <v>284</v>
       </c>
     </row>
     <row r="21">
@@ -4472,19 +4534,22 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>103</v>
+        <v>236</v>
       </c>
       <c r="C21" t="n">
-        <v>150</v>
+        <v>4</v>
       </c>
       <c r="D21" t="n">
+        <v>8</v>
+      </c>
+      <c r="E21" t="n">
         <v>12</v>
       </c>
-      <c r="E21" t="n">
+      <c r="F21" t="n">
         <v>24</v>
       </c>
-      <c r="F21" t="n">
-        <v>289</v>
+      <c r="G21" t="n">
+        <v>284</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v4 modificación de la tabla pivote con incrementos
</commit_message>
<xml_diff>
--- a/salida/excel/consumo_horas_educacion_secundaria.xlsx
+++ b/salida/excel/consumo_horas_educacion_secundaria.xlsx
@@ -4007,7 +4007,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4028,32 +4028,67 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Aula_Incremento</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Laboratorio de Computadoras</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Laboratorio de Computadoras_Incremento</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Laboratorio de Física</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Laboratorio de Física_Incremento</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Laboratorio de Química</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Laboratorio de Química_Incremento</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Taller</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Taller_Incremento</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Virtual</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Virtual_Incremento</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Total</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Total_Incremento</t>
         </is>
       </c>
     </row>
@@ -4067,7 +4102,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -4076,12 +4111,33 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
         <v>4</v>
       </c>
-      <c r="G2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" t="n">
+      <c r="K2" t="n">
+        <v>4</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" t="n">
+        <v>8</v>
+      </c>
+      <c r="O2" t="n">
         <v>8</v>
       </c>
     </row>
@@ -4095,22 +4151,43 @@
         <v>26</v>
       </c>
       <c r="C3" t="n">
+        <v>22</v>
+      </c>
+      <c r="D3" t="n">
         <v>4</v>
       </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
         <v>4</v>
       </c>
-      <c r="G3" t="n">
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
         <v>3</v>
       </c>
-      <c r="H3" t="n">
+      <c r="M3" t="n">
+        <v>3</v>
+      </c>
+      <c r="N3" t="n">
         <v>37</v>
+      </c>
+      <c r="O3" t="n">
+        <v>29</v>
       </c>
     </row>
     <row r="4">
@@ -4123,22 +4200,43 @@
         <v>40</v>
       </c>
       <c r="C4" t="n">
+        <v>14</v>
+      </c>
+      <c r="D4" t="n">
         <v>4</v>
       </c>
-      <c r="D4" t="n">
-        <v>0</v>
-      </c>
       <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
         <v>3</v>
       </c>
-      <c r="F4" t="n">
+      <c r="I4" t="n">
+        <v>3</v>
+      </c>
+      <c r="J4" t="n">
         <v>8</v>
       </c>
-      <c r="G4" t="n">
+      <c r="K4" t="n">
+        <v>4</v>
+      </c>
+      <c r="L4" t="n">
         <v>8</v>
       </c>
-      <c r="H4" t="n">
+      <c r="M4" t="n">
+        <v>5</v>
+      </c>
+      <c r="N4" t="n">
         <v>63</v>
+      </c>
+      <c r="O4" t="n">
+        <v>26</v>
       </c>
     </row>
     <row r="5">
@@ -4151,22 +4249,43 @@
         <v>61</v>
       </c>
       <c r="C5" t="n">
+        <v>21</v>
+      </c>
+      <c r="D5" t="n">
         <v>4</v>
       </c>
-      <c r="D5" t="n">
-        <v>0</v>
-      </c>
       <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
         <v>5</v>
       </c>
-      <c r="F5" t="n">
+      <c r="I5" t="n">
+        <v>2</v>
+      </c>
+      <c r="J5" t="n">
         <v>8</v>
       </c>
-      <c r="G5" t="n">
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
         <v>13</v>
       </c>
-      <c r="H5" t="n">
+      <c r="M5" t="n">
+        <v>5</v>
+      </c>
+      <c r="N5" t="n">
         <v>91</v>
+      </c>
+      <c r="O5" t="n">
+        <v>28</v>
       </c>
     </row>
     <row r="6">
@@ -4179,22 +4298,43 @@
         <v>79</v>
       </c>
       <c r="C6" t="n">
+        <v>18</v>
+      </c>
+      <c r="D6" t="n">
         <v>4</v>
       </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
       <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
         <v>7</v>
       </c>
-      <c r="F6" t="n">
+      <c r="I6" t="n">
+        <v>2</v>
+      </c>
+      <c r="J6" t="n">
         <v>8</v>
       </c>
-      <c r="G6" t="n">
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" t="n">
         <v>13</v>
       </c>
-      <c r="H6" t="n">
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="n">
         <v>111</v>
+      </c>
+      <c r="O6" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="7">
@@ -4207,22 +4347,43 @@
         <v>111</v>
       </c>
       <c r="C7" t="n">
+        <v>32</v>
+      </c>
+      <c r="D7" t="n">
         <v>7</v>
       </c>
-      <c r="D7" t="n">
+      <c r="E7" t="n">
+        <v>3</v>
+      </c>
+      <c r="F7" t="n">
         <v>5</v>
       </c>
-      <c r="E7" t="n">
+      <c r="G7" t="n">
+        <v>5</v>
+      </c>
+      <c r="H7" t="n">
         <v>10</v>
       </c>
-      <c r="F7" t="n">
+      <c r="I7" t="n">
+        <v>3</v>
+      </c>
+      <c r="J7" t="n">
         <v>8</v>
       </c>
-      <c r="G7" t="n">
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
         <v>16</v>
       </c>
-      <c r="H7" t="n">
+      <c r="M7" t="n">
+        <v>3</v>
+      </c>
+      <c r="N7" t="n">
         <v>157</v>
+      </c>
+      <c r="O7" t="n">
+        <v>46</v>
       </c>
     </row>
     <row r="8">
@@ -4235,22 +4396,43 @@
         <v>137</v>
       </c>
       <c r="C8" t="n">
+        <v>26</v>
+      </c>
+      <c r="D8" t="n">
         <v>7</v>
       </c>
-      <c r="D8" t="n">
-        <v>8</v>
-      </c>
       <c r="E8" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
         <v>8</v>
       </c>
       <c r="G8" t="n">
+        <v>3</v>
+      </c>
+      <c r="H8" t="n">
+        <v>10</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>8</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
         <v>16</v>
       </c>
-      <c r="H8" t="n">
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" t="n">
         <v>186</v>
+      </c>
+      <c r="O8" t="n">
+        <v>29</v>
       </c>
     </row>
     <row r="9">
@@ -4263,22 +4445,43 @@
         <v>149</v>
       </c>
       <c r="C9" t="n">
+        <v>12</v>
+      </c>
+      <c r="D9" t="n">
         <v>7</v>
       </c>
-      <c r="D9" t="n">
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
         <v>8</v>
       </c>
-      <c r="E9" t="n">
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
         <v>13</v>
       </c>
-      <c r="F9" t="n">
+      <c r="I9" t="n">
+        <v>3</v>
+      </c>
+      <c r="J9" t="n">
         <v>12</v>
       </c>
-      <c r="G9" t="n">
+      <c r="K9" t="n">
+        <v>4</v>
+      </c>
+      <c r="L9" t="n">
         <v>16</v>
       </c>
-      <c r="H9" t="n">
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" t="n">
         <v>205</v>
+      </c>
+      <c r="O9" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="10">
@@ -4291,22 +4494,43 @@
         <v>181</v>
       </c>
       <c r="C10" t="n">
+        <v>32</v>
+      </c>
+      <c r="D10" t="n">
         <v>7</v>
       </c>
-      <c r="D10" t="n">
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
         <v>8</v>
       </c>
-      <c r="E10" t="n">
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
         <v>13</v>
       </c>
-      <c r="F10" t="n">
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
         <v>12</v>
       </c>
-      <c r="G10" t="n">
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" t="n">
         <v>20</v>
       </c>
-      <c r="H10" t="n">
+      <c r="M10" t="n">
+        <v>4</v>
+      </c>
+      <c r="N10" t="n">
         <v>241</v>
+      </c>
+      <c r="O10" t="n">
+        <v>36</v>
       </c>
     </row>
     <row r="11">
@@ -4319,22 +4543,43 @@
         <v>221</v>
       </c>
       <c r="C11" t="n">
+        <v>40</v>
+      </c>
+      <c r="D11" t="n">
         <v>7</v>
       </c>
-      <c r="D11" t="n">
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
         <v>8</v>
       </c>
-      <c r="E11" t="n">
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
         <v>13</v>
       </c>
-      <c r="F11" t="n">
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
         <v>12</v>
       </c>
-      <c r="G11" t="n">
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" t="n">
         <v>24</v>
       </c>
-      <c r="H11" t="n">
+      <c r="M11" t="n">
+        <v>4</v>
+      </c>
+      <c r="N11" t="n">
         <v>285</v>
+      </c>
+      <c r="O11" t="n">
+        <v>44</v>
       </c>
     </row>
     <row r="12">
@@ -4347,22 +4592,43 @@
         <v>221</v>
       </c>
       <c r="C12" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" t="n">
         <v>7</v>
       </c>
-      <c r="D12" t="n">
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="n">
         <v>8</v>
       </c>
-      <c r="E12" t="n">
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
         <v>13</v>
       </c>
-      <c r="F12" t="n">
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="n">
         <v>12</v>
       </c>
-      <c r="G12" t="n">
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
         <v>24</v>
       </c>
-      <c r="H12" t="n">
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" t="n">
         <v>285</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -4375,22 +4641,43 @@
         <v>221</v>
       </c>
       <c r="C13" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" t="n">
         <v>7</v>
       </c>
-      <c r="D13" t="n">
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="n">
         <v>8</v>
       </c>
-      <c r="E13" t="n">
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="n">
         <v>13</v>
       </c>
-      <c r="F13" t="n">
+      <c r="I13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" t="n">
         <v>12</v>
       </c>
-      <c r="G13" t="n">
+      <c r="K13" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" t="n">
         <v>24</v>
       </c>
-      <c r="H13" t="n">
+      <c r="M13" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" t="n">
         <v>285</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -4403,22 +4690,43 @@
         <v>221</v>
       </c>
       <c r="C14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" t="n">
         <v>7</v>
       </c>
-      <c r="D14" t="n">
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="n">
         <v>8</v>
       </c>
-      <c r="E14" t="n">
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="n">
         <v>13</v>
       </c>
-      <c r="F14" t="n">
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="n">
         <v>12</v>
       </c>
-      <c r="G14" t="n">
+      <c r="K14" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" t="n">
         <v>24</v>
       </c>
-      <c r="H14" t="n">
+      <c r="M14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" t="n">
         <v>285</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -4431,22 +4739,43 @@
         <v>221</v>
       </c>
       <c r="C15" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" t="n">
         <v>7</v>
       </c>
-      <c r="D15" t="n">
+      <c r="E15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" t="n">
         <v>8</v>
       </c>
-      <c r="E15" t="n">
+      <c r="G15" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" t="n">
         <v>13</v>
       </c>
-      <c r="F15" t="n">
+      <c r="I15" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" t="n">
         <v>12</v>
       </c>
-      <c r="G15" t="n">
+      <c r="K15" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" t="n">
         <v>24</v>
       </c>
-      <c r="H15" t="n">
+      <c r="M15" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" t="n">
         <v>285</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -4459,22 +4788,43 @@
         <v>221</v>
       </c>
       <c r="C16" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" t="n">
         <v>7</v>
       </c>
-      <c r="D16" t="n">
+      <c r="E16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" t="n">
         <v>8</v>
       </c>
-      <c r="E16" t="n">
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" t="n">
         <v>13</v>
       </c>
-      <c r="F16" t="n">
+      <c r="I16" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" t="n">
         <v>12</v>
       </c>
-      <c r="G16" t="n">
+      <c r="K16" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" t="n">
         <v>24</v>
       </c>
-      <c r="H16" t="n">
+      <c r="M16" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" t="n">
         <v>285</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -4487,22 +4837,43 @@
         <v>221</v>
       </c>
       <c r="C17" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" t="n">
         <v>7</v>
       </c>
-      <c r="D17" t="n">
+      <c r="E17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" t="n">
         <v>8</v>
       </c>
-      <c r="E17" t="n">
+      <c r="G17" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" t="n">
         <v>13</v>
       </c>
-      <c r="F17" t="n">
+      <c r="I17" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" t="n">
         <v>12</v>
       </c>
-      <c r="G17" t="n">
+      <c r="K17" t="n">
+        <v>0</v>
+      </c>
+      <c r="L17" t="n">
         <v>24</v>
       </c>
-      <c r="H17" t="n">
+      <c r="M17" t="n">
+        <v>0</v>
+      </c>
+      <c r="N17" t="n">
         <v>285</v>
+      </c>
+      <c r="O17" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -4515,22 +4886,43 @@
         <v>221</v>
       </c>
       <c r="C18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" t="n">
         <v>7</v>
       </c>
-      <c r="D18" t="n">
+      <c r="E18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" t="n">
         <v>8</v>
       </c>
-      <c r="E18" t="n">
+      <c r="G18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" t="n">
         <v>13</v>
       </c>
-      <c r="F18" t="n">
+      <c r="I18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" t="n">
         <v>12</v>
       </c>
-      <c r="G18" t="n">
+      <c r="K18" t="n">
+        <v>0</v>
+      </c>
+      <c r="L18" t="n">
         <v>24</v>
       </c>
-      <c r="H18" t="n">
+      <c r="M18" t="n">
+        <v>0</v>
+      </c>
+      <c r="N18" t="n">
         <v>285</v>
+      </c>
+      <c r="O18" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -4543,22 +4935,43 @@
         <v>221</v>
       </c>
       <c r="C19" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" t="n">
         <v>7</v>
       </c>
-      <c r="D19" t="n">
+      <c r="E19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" t="n">
         <v>8</v>
       </c>
-      <c r="E19" t="n">
+      <c r="G19" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" t="n">
         <v>13</v>
       </c>
-      <c r="F19" t="n">
+      <c r="I19" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" t="n">
         <v>12</v>
       </c>
-      <c r="G19" t="n">
+      <c r="K19" t="n">
+        <v>0</v>
+      </c>
+      <c r="L19" t="n">
         <v>24</v>
       </c>
-      <c r="H19" t="n">
+      <c r="M19" t="n">
+        <v>0</v>
+      </c>
+      <c r="N19" t="n">
         <v>285</v>
+      </c>
+      <c r="O19" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -4571,22 +4984,43 @@
         <v>221</v>
       </c>
       <c r="C20" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" t="n">
         <v>7</v>
       </c>
-      <c r="D20" t="n">
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" t="n">
         <v>8</v>
       </c>
-      <c r="E20" t="n">
+      <c r="G20" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" t="n">
         <v>13</v>
       </c>
-      <c r="F20" t="n">
+      <c r="I20" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" t="n">
         <v>12</v>
       </c>
-      <c r="G20" t="n">
+      <c r="K20" t="n">
+        <v>0</v>
+      </c>
+      <c r="L20" t="n">
         <v>24</v>
       </c>
-      <c r="H20" t="n">
+      <c r="M20" t="n">
+        <v>0</v>
+      </c>
+      <c r="N20" t="n">
         <v>285</v>
+      </c>
+      <c r="O20" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -4599,22 +5033,43 @@
         <v>221</v>
       </c>
       <c r="C21" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" t="n">
         <v>7</v>
       </c>
-      <c r="D21" t="n">
+      <c r="E21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" t="n">
         <v>8</v>
       </c>
-      <c r="E21" t="n">
+      <c r="G21" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" t="n">
         <v>13</v>
       </c>
-      <c r="F21" t="n">
+      <c r="I21" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" t="n">
         <v>12</v>
       </c>
-      <c r="G21" t="n">
+      <c r="K21" t="n">
+        <v>0</v>
+      </c>
+      <c r="L21" t="n">
         <v>24</v>
       </c>
-      <c r="H21" t="n">
+      <c r="M21" t="n">
+        <v>0</v>
+      </c>
+      <c r="N21" t="n">
         <v>285</v>
+      </c>
+      <c r="O21" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>